<commit_message>
Update 6-) Dunyada tekstilde en buyuk ihracatcilar ve ithalatcilar.xlsx
</commit_message>
<xml_diff>
--- a/6-) Dunyada tekstilde en buyuk ihracatcilar ve ithalatcilar.xlsx
+++ b/6-) Dunyada tekstilde en buyuk ihracatcilar ve ithalatcilar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fintegral365-my.sharepoint.com/personal/oguz_oztekin_fintegral_com_tr/Documents/Masaüstü/Dis-Ticaret-Tekstil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_26A707F2C0A7F82722E19EC2F73DFDAEE557DCBC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5456C408-7B2A-4D08-B538-DAACF3AD8765}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_26A707F2C0A7F82722E19EC2F73DFDAEE557DCBC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABAA1A04-D2CD-4C63-B82C-DD160C226133}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="0" windowWidth="9885" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15030" yWindow="885" windowWidth="12420" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2012_İhracat" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -5693,9 +5693,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>